<commit_message>
Update PLANO DEL SISTEMA- CINE2.xlsx
</commit_message>
<xml_diff>
--- a/PLANO DEL SISTEMA- CINE2.xlsx
+++ b/PLANO DEL SISTEMA- CINE2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f87ca329e5780eae/Documentos/GitHub/Simulaci-n-de-Cinepolis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{44F4F207-FB4D-4BB8-A485-F0C42FC1DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E63A294-2927-4192-B521-1B2A3F05445F}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{44F4F207-FB4D-4BB8-A485-F0C42FC1DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBE3CEC1-E61E-47AD-AE9B-3312276B7E4B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="73">
   <si>
     <t>DULCERIA</t>
   </si>
@@ -585,6 +585,18 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,19 +606,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X100" sqref="X100"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1287,19 +1287,19 @@
       <c r="BI1" s="1"/>
     </row>
     <row r="2" spans="4:68" ht="14.25" customHeight="1">
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
@@ -1357,52 +1357,52 @@
       <c r="N3" s="2">
         <v>11</v>
       </c>
-      <c r="U3" s="50" t="s">
+      <c r="U3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="61"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
-      <c r="AD3" s="50" t="s">
+      <c r="AD3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="57"/>
-      <c r="AN3" s="50" t="s">
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="57"/>
+      <c r="AJ3" s="61"/>
+      <c r="AN3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="AO3" s="51"/>
-      <c r="AP3" s="51"/>
-      <c r="AQ3" s="51"/>
-      <c r="AR3" s="51"/>
-      <c r="AS3" s="57"/>
-      <c r="AW3" s="50" t="s">
+      <c r="AO3" s="57"/>
+      <c r="AP3" s="57"/>
+      <c r="AQ3" s="57"/>
+      <c r="AR3" s="57"/>
+      <c r="AS3" s="61"/>
+      <c r="AW3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="51"/>
-      <c r="AZ3" s="51"/>
-      <c r="BA3" s="57"/>
-      <c r="BE3" s="50" t="s">
+      <c r="AX3" s="57"/>
+      <c r="AY3" s="57"/>
+      <c r="AZ3" s="57"/>
+      <c r="BA3" s="61"/>
+      <c r="BE3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="BF3" s="51"/>
-      <c r="BG3" s="51"/>
-      <c r="BH3" s="51"/>
-      <c r="BI3" s="52"/>
+      <c r="BF3" s="57"/>
+      <c r="BG3" s="57"/>
+      <c r="BH3" s="57"/>
+      <c r="BI3" s="58"/>
       <c r="BJ3" s="44"/>
       <c r="BK3" s="33"/>
-      <c r="BL3" s="53"/>
-      <c r="BM3" s="54"/>
-      <c r="BN3" s="54"/>
+      <c r="BL3" s="59"/>
+      <c r="BM3" s="60"/>
+      <c r="BN3" s="60"/>
       <c r="BO3" s="33"/>
       <c r="BP3" s="33"/>
     </row>
@@ -1792,12 +1792,12 @@
       <c r="BP6" s="33"/>
     </row>
     <row r="7" spans="4:68" ht="14.25" customHeight="1">
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
       <c r="T7" s="7">
         <v>3</v>
       </c>
@@ -3406,11 +3406,11 @@
       <c r="BP17" s="33"/>
     </row>
     <row r="18" spans="1:68" ht="14.25" customHeight="1">
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
       <c r="Q18" s="3" t="s">
         <v>1</v>
       </c>
@@ -3707,12 +3707,12 @@
     </row>
     <row r="20" spans="1:68" ht="14.25" customHeight="1">
       <c r="D20" s="23"/>
-      <c r="L20" s="58" t="s">
+      <c r="L20" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
       <c r="Q20" s="3"/>
       <c r="T20" s="7">
         <v>16</v>
@@ -5045,14 +5045,14 @@
       <c r="BP28" s="33"/>
     </row>
     <row r="29" spans="1:68" ht="14.25" customHeight="1">
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
       <c r="M29" s="23"/>
       <c r="O29" s="23"/>
       <c r="Q29" s="3"/>
@@ -5200,7 +5200,7 @@
       <c r="BP29" s="33"/>
     </row>
     <row r="30" spans="1:68" ht="14.25" customHeight="1">
-      <c r="B30" s="61"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -6465,7 +6465,7 @@
       <c r="BH64" s="1"/>
       <c r="BI64" s="1"/>
     </row>
-    <row r="65" spans="17:61" ht="14.25" customHeight="1">
+    <row r="65" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF65" s="1"/>
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
@@ -6478,7 +6478,7 @@
       <c r="BH65" s="1"/>
       <c r="BI65" s="1"/>
     </row>
-    <row r="66" spans="17:61" ht="14.25" customHeight="1">
+    <row r="66" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF66" s="1"/>
       <c r="AG66" s="1"/>
       <c r="AH66" s="1"/>
@@ -6491,7 +6491,7 @@
       <c r="BH66" s="1"/>
       <c r="BI66" s="1"/>
     </row>
-    <row r="67" spans="17:61" ht="14.25" customHeight="1">
+    <row r="67" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF67" s="1"/>
       <c r="AG67" s="1"/>
       <c r="AH67" s="1"/>
@@ -6504,7 +6504,7 @@
       <c r="BH67" s="1"/>
       <c r="BI67" s="1"/>
     </row>
-    <row r="68" spans="17:61" ht="14.25" customHeight="1">
+    <row r="68" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF68" s="1"/>
       <c r="AG68" s="1"/>
       <c r="AH68" s="1"/>
@@ -6517,7 +6517,7 @@
       <c r="BH68" s="1"/>
       <c r="BI68" s="1"/>
     </row>
-    <row r="69" spans="17:61" ht="14.25" customHeight="1">
+    <row r="69" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF69" s="1"/>
       <c r="AG69" s="1"/>
       <c r="AH69" s="1"/>
@@ -6530,7 +6530,7 @@
       <c r="BH69" s="1"/>
       <c r="BI69" s="1"/>
     </row>
-    <row r="70" spans="17:61" ht="14.25" customHeight="1">
+    <row r="70" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF70" s="1"/>
       <c r="AG70" s="1"/>
       <c r="AH70" s="1"/>
@@ -6543,7 +6543,7 @@
       <c r="BH70" s="1"/>
       <c r="BI70" s="1"/>
     </row>
-    <row r="71" spans="17:61" ht="14.25" customHeight="1">
+    <row r="71" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF71" s="1"/>
       <c r="AG71" s="1"/>
       <c r="AH71" s="1"/>
@@ -6556,7 +6556,7 @@
       <c r="BH71" s="1"/>
       <c r="BI71" s="1"/>
     </row>
-    <row r="72" spans="17:61" ht="14.25" customHeight="1">
+    <row r="72" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF72" s="1"/>
       <c r="AG72" s="1"/>
       <c r="AH72" s="1"/>
@@ -6569,7 +6569,7 @@
       <c r="BH72" s="1"/>
       <c r="BI72" s="1"/>
     </row>
-    <row r="73" spans="17:61" ht="14.25" customHeight="1">
+    <row r="73" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF73" s="1"/>
       <c r="AG73" s="1"/>
       <c r="AH73" s="1"/>
@@ -6582,7 +6582,7 @@
       <c r="BH73" s="1"/>
       <c r="BI73" s="1"/>
     </row>
-    <row r="74" spans="17:61" ht="14.25" customHeight="1">
+    <row r="74" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF74" s="1"/>
       <c r="AG74" s="1"/>
       <c r="AH74" s="1"/>
@@ -6595,7 +6595,7 @@
       <c r="BH74" s="1"/>
       <c r="BI74" s="1"/>
     </row>
-    <row r="75" spans="17:61" ht="14.25" customHeight="1">
+    <row r="75" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF75" s="1"/>
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
@@ -6608,7 +6608,7 @@
       <c r="BH75" s="1"/>
       <c r="BI75" s="1"/>
     </row>
-    <row r="76" spans="17:61" ht="14.25" customHeight="1">
+    <row r="76" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF76" s="1"/>
       <c r="AG76" s="1"/>
       <c r="AH76" s="1"/>
@@ -6621,7 +6621,7 @@
       <c r="BH76" s="1"/>
       <c r="BI76" s="1"/>
     </row>
-    <row r="77" spans="17:61" ht="14.25" customHeight="1">
+    <row r="77" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF77" s="1"/>
       <c r="AG77" s="1"/>
       <c r="AH77" s="1"/>
@@ -6634,7 +6634,7 @@
       <c r="BH77" s="1"/>
       <c r="BI77" s="1"/>
     </row>
-    <row r="78" spans="17:61" ht="14.25" customHeight="1">
+    <row r="78" spans="6:61" ht="14.25" customHeight="1">
       <c r="Q78" t="s">
         <v>64</v>
       </c>
@@ -6650,7 +6650,26 @@
       <c r="BH78" s="1"/>
       <c r="BI78" s="1"/>
     </row>
-    <row r="79" spans="17:61" ht="14.25" customHeight="1">
+    <row r="79" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79">
+        <v>7</v>
+      </c>
+      <c r="J79" s="37">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="K79" s="37">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L79">
+        <f>(H79*100)/251</f>
+        <v>2.7888446215139444</v>
+      </c>
       <c r="S79">
         <v>1</v>
       </c>
@@ -6679,7 +6698,27 @@
       <c r="BH79" s="1"/>
       <c r="BI79" s="1"/>
     </row>
-    <row r="80" spans="17:61" ht="14.25" customHeight="1">
+    <row r="80" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F80">
+        <v>2</v>
+      </c>
+      <c r="G80" t="s">
+        <v>33</v>
+      </c>
+      <c r="H80">
+        <v>17</v>
+      </c>
+      <c r="J80" s="37">
+        <f>K79</f>
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="K80" s="37">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="L80">
+        <f>(H80*I112)/H112</f>
+        <v>6.7729083665338647</v>
+      </c>
       <c r="S80">
         <v>2</v>
       </c>
@@ -6708,7 +6747,27 @@
       <c r="BH80" s="1"/>
       <c r="BI80" s="1"/>
     </row>
-    <row r="81" spans="19:61" ht="14.25" customHeight="1">
+    <row r="81" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F81">
+        <v>3</v>
+      </c>
+      <c r="G81" t="s">
+        <v>34</v>
+      </c>
+      <c r="H81">
+        <v>7</v>
+      </c>
+      <c r="J81" s="37">
+        <f t="shared" ref="J81:J108" si="10">K80</f>
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="K81" s="37">
+        <v>0.30555555555555602</v>
+      </c>
+      <c r="L81">
+        <f>(H81*100)/251</f>
+        <v>2.7888446215139444</v>
+      </c>
       <c r="S81">
         <v>3</v>
       </c>
@@ -6730,7 +6789,27 @@
       <c r="BH81" s="1"/>
       <c r="BI81" s="1"/>
     </row>
-    <row r="82" spans="19:61" ht="14.25" customHeight="1">
+    <row r="82" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F82">
+        <v>4</v>
+      </c>
+      <c r="G82" t="s">
+        <v>35</v>
+      </c>
+      <c r="H82">
+        <v>10</v>
+      </c>
+      <c r="J82" s="37">
+        <f t="shared" si="10"/>
+        <v>0.30555555555555602</v>
+      </c>
+      <c r="K82" s="37">
+        <v>0.30902777777777801</v>
+      </c>
+      <c r="L82">
+        <f t="shared" ref="L82:L108" si="11">(H82*100)/251</f>
+        <v>3.9840637450199203</v>
+      </c>
       <c r="S82">
         <v>4</v>
       </c>
@@ -6769,7 +6848,27 @@
       <c r="BH82" s="1"/>
       <c r="BI82" s="1"/>
     </row>
-    <row r="83" spans="19:61" ht="14.25" customHeight="1">
+    <row r="83" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F83">
+        <v>5</v>
+      </c>
+      <c r="G83" t="s">
+        <v>36</v>
+      </c>
+      <c r="H83">
+        <v>5</v>
+      </c>
+      <c r="J83" s="37">
+        <f t="shared" si="10"/>
+        <v>0.30902777777777801</v>
+      </c>
+      <c r="K83" s="37">
+        <v>0.3125</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="11"/>
+        <v>1.9920318725099602</v>
+      </c>
       <c r="S83">
         <v>5</v>
       </c>
@@ -6805,7 +6904,27 @@
       <c r="BH83" s="1"/>
       <c r="BI83" s="1"/>
     </row>
-    <row r="84" spans="19:61" ht="14.25" customHeight="1">
+    <row r="84" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F84">
+        <v>6</v>
+      </c>
+      <c r="G84" t="s">
+        <v>37</v>
+      </c>
+      <c r="H84">
+        <v>14</v>
+      </c>
+      <c r="J84" s="37">
+        <f t="shared" si="10"/>
+        <v>0.3125</v>
+      </c>
+      <c r="K84" s="37">
+        <v>0.31597222222222199</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="11"/>
+        <v>5.5776892430278888</v>
+      </c>
       <c r="S84">
         <v>6</v>
       </c>
@@ -6836,7 +6955,27 @@
       <c r="BH84" s="1"/>
       <c r="BI84" s="1"/>
     </row>
-    <row r="85" spans="19:61" ht="14.25" customHeight="1">
+    <row r="85" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F85">
+        <v>7</v>
+      </c>
+      <c r="G85" t="s">
+        <v>38</v>
+      </c>
+      <c r="H85">
+        <v>4</v>
+      </c>
+      <c r="J85" s="37">
+        <f t="shared" si="10"/>
+        <v>0.31597222222222199</v>
+      </c>
+      <c r="K85" s="37">
+        <v>0.31944444444444398</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="11"/>
+        <v>1.593625498007968</v>
+      </c>
       <c r="S85">
         <v>7</v>
       </c>
@@ -6867,7 +7006,27 @@
       <c r="BH85" s="1"/>
       <c r="BI85" s="1"/>
     </row>
-    <row r="86" spans="19:61" ht="14.25" customHeight="1">
+    <row r="86" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F86">
+        <v>8</v>
+      </c>
+      <c r="G86" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H86">
+        <v>8</v>
+      </c>
+      <c r="J86" s="37">
+        <f t="shared" si="10"/>
+        <v>0.31944444444444398</v>
+      </c>
+      <c r="K86" s="37">
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="11"/>
+        <v>3.1872509960159361</v>
+      </c>
       <c r="S86">
         <v>8</v>
       </c>
@@ -6898,7 +7057,27 @@
       <c r="BH86" s="1"/>
       <c r="BI86" s="1"/>
     </row>
-    <row r="87" spans="19:61" ht="14.25" customHeight="1">
+    <row r="87" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F87">
+        <v>9</v>
+      </c>
+      <c r="G87" t="s">
+        <v>40</v>
+      </c>
+      <c r="H87">
+        <v>8</v>
+      </c>
+      <c r="J87" s="37">
+        <f t="shared" si="10"/>
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="K87" s="37">
+        <v>0.32638888888888901</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="11"/>
+        <v>3.1872509960159361</v>
+      </c>
       <c r="S87">
         <v>9</v>
       </c>
@@ -6929,7 +7108,27 @@
       <c r="BH87" s="1"/>
       <c r="BI87" s="1"/>
     </row>
-    <row r="88" spans="19:61" ht="14.25" customHeight="1">
+    <row r="88" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F88">
+        <v>10</v>
+      </c>
+      <c r="G88" t="s">
+        <v>41</v>
+      </c>
+      <c r="H88">
+        <v>7</v>
+      </c>
+      <c r="J88" s="37">
+        <f t="shared" si="10"/>
+        <v>0.32638888888888901</v>
+      </c>
+      <c r="K88" s="37">
+        <v>0.32986111111111099</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="11"/>
+        <v>2.7888446215139444</v>
+      </c>
       <c r="S88">
         <v>10</v>
       </c>
@@ -6960,7 +7159,27 @@
       <c r="BH88" s="1"/>
       <c r="BI88" s="1"/>
     </row>
-    <row r="89" spans="19:61" ht="14.25" customHeight="1">
+    <row r="89" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F89">
+        <v>11</v>
+      </c>
+      <c r="G89" t="s">
+        <v>42</v>
+      </c>
+      <c r="H89">
+        <v>10</v>
+      </c>
+      <c r="J89" s="37">
+        <f t="shared" si="10"/>
+        <v>0.32986111111111099</v>
+      </c>
+      <c r="K89" s="37">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="11"/>
+        <v>3.9840637450199203</v>
+      </c>
       <c r="S89">
         <v>11</v>
       </c>
@@ -6991,7 +7210,27 @@
       <c r="BH89" s="1"/>
       <c r="BI89" s="1"/>
     </row>
-    <row r="90" spans="19:61" ht="14.25" customHeight="1">
+    <row r="90" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F90">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>43</v>
+      </c>
+      <c r="H90">
+        <v>12</v>
+      </c>
+      <c r="J90" s="37">
+        <f t="shared" si="10"/>
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="K90" s="37">
+        <v>0.33680555555555503</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="11"/>
+        <v>4.7808764940239046</v>
+      </c>
       <c r="S90">
         <v>12</v>
       </c>
@@ -7022,7 +7261,27 @@
       <c r="BH90" s="1"/>
       <c r="BI90" s="1"/>
     </row>
-    <row r="91" spans="19:61" ht="14.25" customHeight="1">
+    <row r="91" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F91">
+        <v>13</v>
+      </c>
+      <c r="G91" t="s">
+        <v>44</v>
+      </c>
+      <c r="H91">
+        <v>7</v>
+      </c>
+      <c r="J91" s="37">
+        <f t="shared" si="10"/>
+        <v>0.33680555555555503</v>
+      </c>
+      <c r="K91" s="37">
+        <v>0.34027777777777801</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="11"/>
+        <v>2.7888446215139444</v>
+      </c>
       <c r="S91">
         <v>13</v>
       </c>
@@ -7053,7 +7312,27 @@
       <c r="BH91" s="1"/>
       <c r="BI91" s="1"/>
     </row>
-    <row r="92" spans="19:61" ht="14.25" customHeight="1">
+    <row r="92" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F92">
+        <v>14</v>
+      </c>
+      <c r="G92" t="s">
+        <v>45</v>
+      </c>
+      <c r="H92">
+        <v>8</v>
+      </c>
+      <c r="J92" s="37">
+        <f t="shared" si="10"/>
+        <v>0.34027777777777801</v>
+      </c>
+      <c r="K92" s="37">
+        <v>0.34375</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="11"/>
+        <v>3.1872509960159361</v>
+      </c>
       <c r="S92">
         <v>14</v>
       </c>
@@ -7084,7 +7363,27 @@
       <c r="BH92" s="1"/>
       <c r="BI92" s="1"/>
     </row>
-    <row r="93" spans="19:61" ht="14.25" customHeight="1">
+    <row r="93" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F93">
+        <v>15</v>
+      </c>
+      <c r="G93" t="s">
+        <v>46</v>
+      </c>
+      <c r="H93">
+        <v>10</v>
+      </c>
+      <c r="J93" s="37">
+        <f t="shared" si="10"/>
+        <v>0.34375</v>
+      </c>
+      <c r="K93" s="37">
+        <v>0.34722222222222199</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="11"/>
+        <v>3.9840637450199203</v>
+      </c>
       <c r="S93">
         <v>15</v>
       </c>
@@ -7115,7 +7414,27 @@
       <c r="BH93" s="1"/>
       <c r="BI93" s="1"/>
     </row>
-    <row r="94" spans="19:61" ht="14.25" customHeight="1">
+    <row r="94" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F94">
+        <v>16</v>
+      </c>
+      <c r="G94" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H94">
+        <v>9</v>
+      </c>
+      <c r="J94" s="37">
+        <f t="shared" si="10"/>
+        <v>0.34722222222222199</v>
+      </c>
+      <c r="K94" s="37">
+        <v>0.35069444444444398</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="11"/>
+        <v>3.5856573705179282</v>
+      </c>
       <c r="S94">
         <v>16</v>
       </c>
@@ -7146,7 +7465,27 @@
       <c r="BH94" s="1"/>
       <c r="BI94" s="1"/>
     </row>
-    <row r="95" spans="19:61" ht="14.25" customHeight="1">
+    <row r="95" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F95">
+        <v>17</v>
+      </c>
+      <c r="G95" t="s">
+        <v>48</v>
+      </c>
+      <c r="H95">
+        <v>12</v>
+      </c>
+      <c r="J95" s="37">
+        <f t="shared" si="10"/>
+        <v>0.35069444444444398</v>
+      </c>
+      <c r="K95" s="37">
+        <v>0.35416666666666702</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="11"/>
+        <v>4.7808764940239046</v>
+      </c>
       <c r="S95">
         <v>17</v>
       </c>
@@ -7177,7 +7516,27 @@
       <c r="BH95" s="1"/>
       <c r="BI95" s="1"/>
     </row>
-    <row r="96" spans="19:61" ht="14.25" customHeight="1">
+    <row r="96" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F96">
+        <v>18</v>
+      </c>
+      <c r="G96" t="s">
+        <v>49</v>
+      </c>
+      <c r="H96">
+        <v>7</v>
+      </c>
+      <c r="J96" s="37">
+        <f t="shared" si="10"/>
+        <v>0.35416666666666702</v>
+      </c>
+      <c r="K96" s="37">
+        <v>0.35763888888888901</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="11"/>
+        <v>2.7888446215139444</v>
+      </c>
       <c r="S96">
         <v>18</v>
       </c>
@@ -7208,7 +7567,27 @@
       <c r="BH96" s="1"/>
       <c r="BI96" s="1"/>
     </row>
-    <row r="97" spans="19:61" ht="14.25" customHeight="1">
+    <row r="97" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F97">
+        <v>19</v>
+      </c>
+      <c r="G97" t="s">
+        <v>50</v>
+      </c>
+      <c r="H97">
+        <v>8</v>
+      </c>
+      <c r="J97" s="37">
+        <f t="shared" si="10"/>
+        <v>0.35763888888888901</v>
+      </c>
+      <c r="K97" s="37">
+        <v>0.36111111111111099</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="11"/>
+        <v>3.1872509960159361</v>
+      </c>
       <c r="S97">
         <v>19</v>
       </c>
@@ -7239,7 +7618,27 @@
       <c r="BH97" s="1"/>
       <c r="BI97" s="1"/>
     </row>
-    <row r="98" spans="19:61" ht="14.25" customHeight="1">
+    <row r="98" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F98">
+        <v>20</v>
+      </c>
+      <c r="G98" t="s">
+        <v>51</v>
+      </c>
+      <c r="H98">
+        <v>10</v>
+      </c>
+      <c r="J98" s="37">
+        <f t="shared" si="10"/>
+        <v>0.36111111111111099</v>
+      </c>
+      <c r="K98" s="37">
+        <v>0.36458333333333298</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="11"/>
+        <v>3.9840637450199203</v>
+      </c>
       <c r="S98">
         <v>20</v>
       </c>
@@ -7270,7 +7669,27 @@
       <c r="BH98" s="1"/>
       <c r="BI98" s="1"/>
     </row>
-    <row r="99" spans="19:61" ht="14.25" customHeight="1">
+    <row r="99" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F99">
+        <v>21</v>
+      </c>
+      <c r="G99" t="s">
+        <v>52</v>
+      </c>
+      <c r="H99">
+        <v>6</v>
+      </c>
+      <c r="J99" s="37">
+        <f t="shared" si="10"/>
+        <v>0.36458333333333298</v>
+      </c>
+      <c r="K99" s="37">
+        <v>0.36805555555555503</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="11"/>
+        <v>2.3904382470119523</v>
+      </c>
       <c r="S99">
         <v>21</v>
       </c>
@@ -7301,7 +7720,27 @@
       <c r="BH99" s="1"/>
       <c r="BI99" s="1"/>
     </row>
-    <row r="100" spans="19:61" ht="14.25" customHeight="1">
+    <row r="100" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F100">
+        <v>22</v>
+      </c>
+      <c r="G100" t="s">
+        <v>53</v>
+      </c>
+      <c r="H100">
+        <v>9</v>
+      </c>
+      <c r="J100" s="37">
+        <f t="shared" si="10"/>
+        <v>0.36805555555555503</v>
+      </c>
+      <c r="K100" s="37">
+        <v>0.37152777777777801</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="11"/>
+        <v>3.5856573705179282</v>
+      </c>
       <c r="S100">
         <v>22</v>
       </c>
@@ -7332,7 +7771,27 @@
       <c r="BH100" s="1"/>
       <c r="BI100" s="1"/>
     </row>
-    <row r="101" spans="19:61" ht="14.25" customHeight="1">
+    <row r="101" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F101">
+        <v>23</v>
+      </c>
+      <c r="G101" t="s">
+        <v>54</v>
+      </c>
+      <c r="H101">
+        <v>5</v>
+      </c>
+      <c r="J101" s="37">
+        <f t="shared" si="10"/>
+        <v>0.37152777777777801</v>
+      </c>
+      <c r="K101" s="37">
+        <v>0.375</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="11"/>
+        <v>1.9920318725099602</v>
+      </c>
       <c r="S101">
         <v>23</v>
       </c>
@@ -7363,7 +7822,27 @@
       <c r="BH101" s="1"/>
       <c r="BI101" s="1"/>
     </row>
-    <row r="102" spans="19:61" ht="14.25" customHeight="1">
+    <row r="102" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F102">
+        <v>24</v>
+      </c>
+      <c r="G102" t="s">
+        <v>55</v>
+      </c>
+      <c r="H102">
+        <v>6</v>
+      </c>
+      <c r="J102" s="37">
+        <f t="shared" si="10"/>
+        <v>0.375</v>
+      </c>
+      <c r="K102" s="37">
+        <v>0.37847222222222199</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="11"/>
+        <v>2.3904382470119523</v>
+      </c>
       <c r="S102">
         <v>24</v>
       </c>
@@ -7394,7 +7873,27 @@
       <c r="BH102" s="1"/>
       <c r="BI102" s="1"/>
     </row>
-    <row r="103" spans="19:61" ht="14.25" customHeight="1">
+    <row r="103" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F103">
+        <v>25</v>
+      </c>
+      <c r="G103" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="H103">
+        <v>8</v>
+      </c>
+      <c r="J103" s="37">
+        <f t="shared" si="10"/>
+        <v>0.37847222222222199</v>
+      </c>
+      <c r="K103" s="37">
+        <v>0.38194444444444398</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="11"/>
+        <v>3.1872509960159361</v>
+      </c>
       <c r="S103">
         <v>25</v>
       </c>
@@ -7425,7 +7924,27 @@
       <c r="BH103" s="1"/>
       <c r="BI103" s="1"/>
     </row>
-    <row r="104" spans="19:61" ht="14.25" customHeight="1">
+    <row r="104" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F104">
+        <v>26</v>
+      </c>
+      <c r="G104" t="s">
+        <v>57</v>
+      </c>
+      <c r="H104">
+        <v>10</v>
+      </c>
+      <c r="J104" s="37">
+        <f t="shared" si="10"/>
+        <v>0.38194444444444398</v>
+      </c>
+      <c r="K104" s="37">
+        <v>0.38541666666666602</v>
+      </c>
+      <c r="L104">
+        <f t="shared" si="11"/>
+        <v>3.9840637450199203</v>
+      </c>
       <c r="S104">
         <v>26</v>
       </c>
@@ -7456,7 +7975,27 @@
       <c r="BH104" s="1"/>
       <c r="BI104" s="1"/>
     </row>
-    <row r="105" spans="19:61" ht="14.25" customHeight="1">
+    <row r="105" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F105">
+        <v>27</v>
+      </c>
+      <c r="G105" t="s">
+        <v>58</v>
+      </c>
+      <c r="H105">
+        <v>7</v>
+      </c>
+      <c r="J105" s="37">
+        <f t="shared" si="10"/>
+        <v>0.38541666666666602</v>
+      </c>
+      <c r="K105" s="37">
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="11"/>
+        <v>2.7888446215139444</v>
+      </c>
       <c r="S105">
         <v>27</v>
       </c>
@@ -7487,7 +8026,27 @@
       <c r="BH105" s="1"/>
       <c r="BI105" s="1"/>
     </row>
-    <row r="106" spans="19:61" ht="14.25" customHeight="1">
+    <row r="106" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F106">
+        <v>28</v>
+      </c>
+      <c r="G106" t="s">
+        <v>59</v>
+      </c>
+      <c r="H106">
+        <v>9</v>
+      </c>
+      <c r="J106" s="37">
+        <f t="shared" si="10"/>
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="K106" s="37">
+        <v>0.39236111111111099</v>
+      </c>
+      <c r="L106">
+        <f t="shared" si="11"/>
+        <v>3.5856573705179282</v>
+      </c>
       <c r="S106">
         <v>28</v>
       </c>
@@ -7518,7 +8077,27 @@
       <c r="BH106" s="1"/>
       <c r="BI106" s="1"/>
     </row>
-    <row r="107" spans="19:61" ht="14.25" customHeight="1">
+    <row r="107" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F107">
+        <v>29</v>
+      </c>
+      <c r="G107" t="s">
+        <v>60</v>
+      </c>
+      <c r="H107">
+        <v>5</v>
+      </c>
+      <c r="J107" s="37">
+        <f t="shared" si="10"/>
+        <v>0.39236111111111099</v>
+      </c>
+      <c r="K107" s="37">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="L107">
+        <f t="shared" si="11"/>
+        <v>1.9920318725099602</v>
+      </c>
       <c r="S107">
         <v>29</v>
       </c>
@@ -7549,7 +8128,27 @@
       <c r="BH107" s="1"/>
       <c r="BI107" s="1"/>
     </row>
-    <row r="108" spans="19:61" ht="14.25" customHeight="1">
+    <row r="108" spans="6:61" ht="14.25" customHeight="1">
+      <c r="F108">
+        <v>30</v>
+      </c>
+      <c r="G108" t="s">
+        <v>61</v>
+      </c>
+      <c r="H108">
+        <v>6</v>
+      </c>
+      <c r="J108" s="37">
+        <f t="shared" si="10"/>
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="K108" s="37">
+        <v>0.39930555555555503</v>
+      </c>
+      <c r="L108">
+        <f t="shared" si="11"/>
+        <v>2.3904382470119523</v>
+      </c>
       <c r="S108">
         <v>30</v>
       </c>
@@ -7580,7 +8179,7 @@
       <c r="BH108" s="1"/>
       <c r="BI108" s="1"/>
     </row>
-    <row r="109" spans="19:61" ht="14.25" customHeight="1">
+    <row r="109" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF109" s="1"/>
       <c r="AG109" s="1"/>
       <c r="AH109" s="1"/>
@@ -7602,7 +8201,7 @@
       <c r="BH109" s="1"/>
       <c r="BI109" s="1"/>
     </row>
-    <row r="110" spans="19:61" ht="14.25" customHeight="1">
+    <row r="110" spans="6:61" ht="14.25" customHeight="1">
       <c r="U110">
         <f>SUM(U79:U109)</f>
         <v>251</v>
@@ -7628,7 +8227,7 @@
       <c r="BH110" s="1"/>
       <c r="BI110" s="1"/>
     </row>
-    <row r="111" spans="19:61" ht="14.25" customHeight="1">
+    <row r="111" spans="6:61" ht="14.25" customHeight="1">
       <c r="AF111" s="1"/>
       <c r="AG111" s="1"/>
       <c r="AH111" s="1"/>
@@ -7650,7 +8249,14 @@
       <c r="BH111" s="1"/>
       <c r="BI111" s="1"/>
     </row>
-    <row r="112" spans="19:61" ht="14.25" customHeight="1">
+    <row r="112" spans="6:61" ht="14.25" customHeight="1">
+      <c r="H112">
+        <f>SUM(H79:H111)</f>
+        <v>251</v>
+      </c>
+      <c r="I112">
+        <v>100</v>
+      </c>
       <c r="AF112" s="1"/>
       <c r="AG112" s="1"/>
       <c r="AH112" s="1"/>
@@ -23313,11 +23919,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:F29"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="BL3:BN3"/>
     <mergeCell ref="D2:N2"/>
@@ -23325,6 +23926,11 @@
     <mergeCell ref="AD3:AJ3"/>
     <mergeCell ref="AN3:AS3"/>
     <mergeCell ref="AW3:BA3"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>